<commit_message>
Make swarm, bland and cms all respect "estimate" and/or "se"
</commit_message>
<xml_diff>
--- a/info/graph structures.xlsx
+++ b/info/graph structures.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ian\git\siman\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FA1844-01E3-4B49-A998-4AAE4ADCEE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15416EF6-CF7E-4456-9361-E88ECA4EC7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="1005" windowWidth="16980" windowHeight="18885" xr2:uid="{A560A40C-6B58-4431-A5CF-FF0A0FD75D05}"/>
+    <workbookView xWindow="5070" yWindow="5175" windowWidth="27675" windowHeight="11235" xr2:uid="{A560A40C-6B58-4431-A5CF-FF0A0FD75D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="for paper" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="56">
   <si>
     <t>Program</t>
   </si>
@@ -74,12 +75,6 @@
     <t>zipplot</t>
   </si>
   <si>
-    <t>dgm*target*method</t>
-  </si>
-  <si>
-    <t>1 or 2: estimate, se or both</t>
-  </si>
-  <si>
     <t>lollyplot</t>
   </si>
   <si>
@@ -98,9 +93,6 @@
     <t>panels (row)</t>
   </si>
   <si>
-    <t>pm*dgm</t>
-  </si>
-  <si>
     <t>stats</t>
   </si>
   <si>
@@ -113,30 +105,18 @@
     <t>combined for 2-3 methods</t>
   </si>
   <si>
-    <t>dgm and target</t>
-  </si>
-  <si>
-    <t>method*method</t>
-  </si>
-  <si>
     <t>x-axis</t>
   </si>
   <si>
     <t>overlay</t>
   </si>
   <si>
-    <t>target and PM</t>
-  </si>
-  <si>
     <t>one</t>
   </si>
   <si>
     <t>one only</t>
   </si>
   <si>
-    <t>default name</t>
-  </si>
-  <si>
     <t>swarm_[estimate|se]</t>
   </si>
   <si>
@@ -146,44 +126,92 @@
     <t>cms_[graphno]</t>
   </si>
   <si>
-    <t>blandaltman_[dgmno]_[target]</t>
-  </si>
-  <si>
     <t>lollyplot or lollyplot_[target]</t>
   </si>
   <si>
-    <t>by option</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>graphs (over)</t>
-  </si>
-  <si>
-    <t>panels (by)</t>
-  </si>
-  <si>
-    <t>within panels</t>
-  </si>
-  <si>
-    <t>dgm*target</t>
-  </si>
-  <si>
     <t>dgms</t>
   </si>
   <si>
     <t>methods</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>One or two: estimate, se or both</t>
+  </si>
+  <si>
+    <t>One per dgm and target</t>
+  </si>
+  <si>
+    <t>One per target</t>
+  </si>
+  <si>
+    <t>One per target and PM</t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>Panels</t>
+  </si>
+  <si>
+    <t>Graph default name</t>
+  </si>
+  <si>
+    <t>blandaltman_[graphno]_[estimate|se]</t>
+  </si>
+  <si>
+    <t>Within panels</t>
+  </si>
+  <si>
+    <t>blandaltman</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>statistic = estimate or se</t>
+  </si>
+  <si>
+    <t>swarm_[statistic]</t>
+  </si>
+  <si>
+    <t>blandaltman_[graphno]_[statistic]</t>
+  </si>
+  <si>
+    <t>dgm, target, method</t>
+  </si>
+  <si>
+    <t>dgm, target</t>
+  </si>
+  <si>
+    <t>pm, dgm</t>
+  </si>
+  <si>
+    <t>method, method</t>
+  </si>
+  <si>
+    <t>dgm, target, statistic</t>
+  </si>
+  <si>
+    <t>target, PM</t>
+  </si>
+  <si>
+    <t>Default graph name</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,16 +232,30 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -232,11 +274,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8EA9DB"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -250,20 +348,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -274,12 +391,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -441,7 +552,7 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <fgColor indexed="64"/>
+          <fgColor rgb="FF000000"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -496,20 +607,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4055C9C6-B9E8-4021-B2D5-76E02871648B}" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K8" xr:uid="{4055C9C6-B9E8-4021-B2D5-76E02871648B}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{9716A1F6-6366-4F4B-87D8-68EDDE7C8A97}" name="Program" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{18590F41-95FB-4075-BBC8-D06143311723}" name="dgm" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{AACF4E5E-48DE-4C05-867B-B33D24689A8E}" name="target" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{1B0A2701-15F6-4F17-AB86-A90F3E349B97}" name="method" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{7C3B4866-402B-42C2-AACD-AC69337F783D}" name="stats" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A8C417F3-CC0E-4B23-A351-EA0B819A342D}" name="PMs" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6CFF1D63-18E4-4D41-AA3C-137C7206B90B}" name="graphs (over)" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F02E275E-FB4E-49D0-A6E4-F6511A9CA7F5}" name="panels (by)" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{9F4BCCB4-790D-44A6-A89D-041381D94286}" name="within panels" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{0AF57FD6-13BB-4D03-8D91-3780F840A769}" name="default name" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{C5CD823B-34D5-42E4-A477-AC6B51A9A9FA}" name="by option" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{02EE9E74-7CCD-4436-A9B9-1F59269C5635}" name="Table13" displayName="Table13" ref="A1:J8" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J8" xr:uid="{4055C9C6-B9E8-4021-B2D5-76E02871648B}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{66D16A24-5FA3-4002-920C-BC0CB6A42DFB}" name="Program" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{5ED0438B-131B-40AF-97C7-58D1151E30CA}" name="dgm" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{42F79FE0-BAA6-4C79-A93D-C7355148C0BD}" name="target" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8892DF8E-C4FE-434F-BE39-B06E849C2769}" name="method" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{D98CD60F-F6A7-4D8E-A010-89B952F87993}" name="stats" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{E5656B08-8953-48E9-BEB8-03683ACB65DF}" name="PMs" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{341AE6A2-4AC8-4AF6-B640-97D3FBCC3A67}" name="Graphs" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{24B6F356-4979-4F23-B954-E849CB611268}" name="Panels" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{0B0A8B4E-B5D2-4BB4-B848-B6A1307DFAC5}" name="Within panels" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{B1223FF2-D9CE-438B-AE3A-CFA9A899EA6D}" name="Graph default name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -832,10 +942,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44914DA-B370-44D6-A3FA-C47E328B7433}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7559712-E29C-4A4B-AF21-552E85F89719}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,10 +1243,10 @@
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -862,28 +1260,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -897,28 +1292,25 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,25 +1327,22 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -967,28 +1356,25 @@
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1002,30 +1388,27 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -1037,33 +1420,30 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
@@ -1072,60 +1452,54 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="J8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>